<commit_message>
feat: Update data input files and improve validation logic; handle duplicates in LPU and NLPU validators
</commit_message>
<xml_diff>
--- a/data/inputs/saude_esteira/BASE_SAUDE_DA_ESTEIRA.xlsx
+++ b/data/inputs/saude_esteira/BASE_SAUDE_DA_ESTEIRA.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/saude_esteira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F235C80-7625-48C0-99EE-7095B595C9EF}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5264A996-6716-4A18-A0DC-3E08CA7CA8DE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="DOCUMENTOS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -427,9 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>